<commit_message>
Adding and data being viewed
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
@@ -80,6 +80,74 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -372,13 +440,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="30" customWidth="1" style="1" min="1" max="1"/>
     <col width="10" customWidth="1" style="1" min="2" max="2"/>
@@ -387,46 +455,112 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>Name of Product</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Quantity in grams</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>No. of pieces</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>MRP</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>hey</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>102</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Ths</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>2312</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Iphone</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>102000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Television</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2132</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>231</t>
         </is>
       </c>
     </row>

</xml_diff>